<commit_message>
die output attention= false weg gehaald want zorgde ervoor dat bert niet meer werkte
</commit_message>
<xml_diff>
--- a/Identifier/Updated_Methodology_Test.xlsx
+++ b/Identifier/Updated_Methodology_Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E51DC13-7F20-4544-BB0B-043AF66051E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8625A071-0127-4EBD-8972-BACACAC84E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1042,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J202"/>
+  <dimension ref="A1:J203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7522,6 +7522,40 @@
         <v>23</v>
       </c>
     </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C203">
+        <f>SUMIFS(C2:C201, C2:C201, 1, $B2:$B201, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="D203">
+        <f t="shared" ref="D203:J203" si="0">SUMIFS(D2:D201, D2:D201, 1, $B2:$B201, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E203">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F203">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G203">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I203">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J203">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>